<commit_message>
Culminacion con los reportes de Anny
</commit_message>
<xml_diff>
--- a/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
+++ b/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Resumen de Desempeño Por Unidad</x:t>
   </x:si>
@@ -46,13 +46,10 @@
     <x:t>Total por unidad:</x:t>
   </x:si>
   <x:si>
-    <x:t>100%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>75%</x:t>
+    <x:t>33%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67%</x:t>
   </x:si>
   <x:si>
     <x:t>Total:</x:t>
@@ -682,7 +679,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E12"/>
+  <x:dimension ref="A1:E13"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -731,13 +728,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C4" s="7" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D4" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="E4" s="9" t="n">
-        <x:v>1000</x:v>
+        <x:v>2000</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -748,13 +745,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C5" s="7" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D5" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="E5" s="9" t="n">
-        <x:v>2300</x:v>
+        <x:v>3100</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
@@ -763,11 +760,11 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C6" s="11" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s"/>
       <x:c r="E6" s="13" t="n">
-        <x:v>3300</x:v>
+        <x:v>5100</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
@@ -775,7 +772,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B7" s="7" t="s">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C7" s="7" t="n">
         <x:v>1</x:v>
@@ -784,37 +781,37 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="E7" s="9" t="n">
-        <x:v>350</x:v>
+        <x:v>365</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
-      <x:c r="A8" s="10" t="s"/>
-      <x:c r="B8" s="11" t="s">
+      <x:c r="A8" s="6" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B8" s="7" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C8" s="7" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D8" s="8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E8" s="9" t="n">
+        <x:v>850</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="A9" s="10" t="s"/>
+      <x:c r="B9" s="11" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C8" s="11" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D8" s="12" t="s"/>
-      <x:c r="E8" s="13" t="n">
-        <x:v>350</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="6" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B9" s="7" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C9" s="7" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D9" s="8" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E9" s="9" t="n">
-        <x:v>400</x:v>
+      <x:c r="C9" s="11" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D9" s="12" t="s"/>
+      <x:c r="E9" s="13" t="n">
+        <x:v>1215</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -825,39 +822,56 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C10" s="7" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D10" s="8" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E10" s="9" t="n">
+        <x:v>4350</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="A11" s="6" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B11" s="7" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C11" s="7" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D11" s="8" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E11" s="9" t="n">
+        <x:v>4455</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="A12" s="14" t="s"/>
+      <x:c r="B12" s="15" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C12" s="15" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D12" s="16" t="s"/>
+      <x:c r="E12" s="17" t="n">
+        <x:v>8805</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5">
+      <x:c r="A13" s="11" t="s"/>
+      <x:c r="B13" s="11" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E10" s="9" t="n">
-        <x:v>2150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="14" t="s"/>
-      <x:c r="B11" s="15" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C11" s="15" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D11" s="16" t="s"/>
-      <x:c r="E11" s="17" t="n">
-        <x:v>2550</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="11" t="s"/>
-      <x:c r="B12" s="11" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C12" s="11" t="n">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D12" s="12" t="s"/>
-      <x:c r="E12" s="18" t="n">
-        <x:v>6200</x:v>
+      <x:c r="C13" s="11" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D13" s="12" t="s"/>
+      <x:c r="E13" s="18" t="n">
+        <x:v>15120</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Completacion de campos nulos, depligue de pendientes a assignar
</commit_message>
<xml_diff>
--- a/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
+++ b/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <x:si>
     <x:t>Resumen de Desempeño Por Unidad</x:t>
   </x:si>
@@ -46,10 +46,16 @@
     <x:t>Total por unidad:</x:t>
   </x:si>
   <x:si>
-    <x:t>33%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>67%</x:t>
+    <x:t>44%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60%</x:t>
   </x:si>
   <x:si>
     <x:t>Total:</x:t>
@@ -61,7 +67,7 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="1" formatCode="#,###"/>
+    <x:numFmt numFmtId="165" formatCode="#,###"/>
   </x:numFmts>
   <x:fonts count="5">
     <x:font>
@@ -221,166 +227,166 @@
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="23">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="23">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -391,7 +397,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -674,7 +680,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -772,16 +778,16 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B7" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C7" s="7" t="n">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="D7" s="8" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="E7" s="9" t="n">
-        <x:v>365</x:v>
+        <x:v>2550</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
@@ -789,16 +795,16 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B8" s="7" t="s">
-        <x:v>8</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C8" s="7" t="n">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D8" s="8" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="E8" s="9" t="n">
-        <x:v>850</x:v>
+        <x:v>4140</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
@@ -807,11 +813,11 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C9" s="11" t="n">
-        <x:v>3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s"/>
       <x:c r="E9" s="13" t="n">
-        <x:v>1215</x:v>
+        <x:v>6690</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -819,16 +825,16 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="B10" s="7" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C10" s="7" t="n">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C10" s="7" t="n">
-        <x:v>5</x:v>
-      </x:c>
       <x:c r="D10" s="8" t="s">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E10" s="9" t="n">
-        <x:v>4350</x:v>
+        <x:v>8440</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -836,16 +842,16 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="B11" s="7" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C11" s="7" t="n">
-        <x:v>5</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D11" s="8" t="s">
-        <x:v>7</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E11" s="9" t="n">
-        <x:v>4455</x:v>
+        <x:v>9735</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -854,24 +860,24 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C12" s="15" t="n">
-        <x:v>10</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D12" s="16" t="s"/>
       <x:c r="E12" s="17" t="n">
-        <x:v>8805</x:v>
+        <x:v>18175</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="11" t="s"/>
       <x:c r="B13" s="11" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C13" s="11" t="n">
-        <x:v>17</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D13" s="12" t="s"/>
       <x:c r="E13" s="18" t="n">
-        <x:v>15120</x:v>
+        <x:v>29965</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Modificacion de los reportes
</commit_message>
<xml_diff>
--- a/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
+++ b/SRAM/Content/Report/73156_reporte Por Unidad.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Resumen de Desempeño Por Unidad</x:t>
   </x:si>
@@ -37,25 +37,22 @@
     <x:t>Inválida</x:t>
   </x:si>
   <x:si>
-    <x:t>50%</x:t>
+    <x:t>40%</x:t>
   </x:si>
   <x:si>
     <x:t>Válida</x:t>
   </x:si>
   <x:si>
+    <x:t>60%</x:t>
+  </x:si>
+  <x:si>
     <x:t>Total por unidad:</x:t>
   </x:si>
   <x:si>
-    <x:t>44%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>56%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>60%</x:t>
+    <x:t>14%</x:t>
+  </x:si>
+  <x:si>
+    <x:t>86%</x:t>
   </x:si>
   <x:si>
     <x:t>Total:</x:t>
@@ -69,7 +66,7 @@
     <x:numFmt numFmtId="0" formatCode=""/>
     <x:numFmt numFmtId="165" formatCode="#,###"/>
   </x:numFmts>
-  <x:fonts count="5">
+  <x:fonts count="6">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -82,21 +79,29 @@
       <x:vertAlign val="baseline"/>
       <x:sz val="14"/>
       <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
+      <x:name val="Cambria"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
+      <x:b/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
-      <x:color rgb="FFFFFFFF"/>
-      <x:name val="Calibri"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Cambria"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FFFF0000"/>
-      <x:name val="Calibri"/>
+      <x:name val="Cambria"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Cambria"/>
       <x:family val="2"/>
     </x:font>
     <x:font>
@@ -108,21 +113,15 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="3">
+  <x:fills count="2">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
     </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FF00008B"/>
-        <x:bgColor rgb="FF00008B"/>
-      </x:patternFill>
-    </x:fill>
   </x:fills>
-  <x:borders count="6">
+  <x:borders count="9">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -142,7 +141,7 @@
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="thick">
-        <x:color rgb="FF00008B"/>
+        <x:color rgb="FF000000"/>
       </x:left>
       <x:right style="none">
         <x:color rgb="FF000000"/>
@@ -150,7 +149,7 @@
       <x:top style="none">
         <x:color rgb="FF000000"/>
       </x:top>
-      <x:bottom style="none">
+      <x:bottom style="thick">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -161,13 +160,30 @@
       <x:left style="none">
         <x:color rgb="FF000000"/>
       </x:left>
-      <x:right style="thick">
-        <x:color rgb="FF00008B"/>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
       </x:right>
       <x:top style="none">
         <x:color rgb="FF000000"/>
       </x:top>
-      <x:bottom style="none">
+      <x:bottom style="thick">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="thick">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thick">
         <x:color rgb="FF000000"/>
       </x:bottom>
       <x:diagonal style="none">
@@ -176,13 +192,47 @@
     </x:border>
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="thick">
-        <x:color rgb="FF00008B"/>
+        <x:color rgb="FF000000"/>
       </x:left>
       <x:right style="none">
         <x:color rgb="FF000000"/>
       </x:right>
       <x:top style="none">
         <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="thick">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="thick">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="thick">
+        <x:color rgb="FF00008B"/>
       </x:top>
       <x:bottom style="thick">
         <x:color rgb="FF00008B"/>
@@ -198,8 +248,8 @@
       <x:right style="none">
         <x:color rgb="FF000000"/>
       </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
+      <x:top style="thick">
+        <x:color rgb="FF00008B"/>
       </x:top>
       <x:bottom style="thick">
         <x:color rgb="FF00008B"/>
@@ -213,10 +263,10 @@
         <x:color rgb="FF000000"/>
       </x:left>
       <x:right style="thick">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="thick">
         <x:color rgb="FF00008B"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
       </x:top>
       <x:bottom style="thick">
         <x:color rgb="FF00008B"/>
@@ -226,26 +276,26 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="23">
+  <x:cellStyleXfs count="25">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -254,10 +304,22 @@
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -266,38 +328,32 @@
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="165" fontId="4" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="23">
+  <x:cellXfs count="25">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -306,23 +362,23 @@
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -334,11 +390,27 @@
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -350,44 +422,36 @@
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -685,7 +749,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E13"/>
+  <x:dimension ref="A1:E10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -693,8 +757,8 @@
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="17.710625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.140625" style="22" customWidth="1"/>
+    <x:col min="3" max="3" width="20.710625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="14.710625" style="23" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5">
@@ -703,13 +767,13 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5">
-      <x:c r="A2" s="20" t="s"/>
-      <x:c r="B2" s="20" t="s"/>
-      <x:c r="C2" s="20" t="s"/>
-      <x:c r="D2" s="21" t="s"/>
-      <x:c r="E2" s="19" t="s"/>
+      <x:c r="A2" s="21" t="s"/>
+      <x:c r="B2" s="21" t="s"/>
+      <x:c r="C2" s="21" t="s"/>
+      <x:c r="D2" s="22" t="s"/>
+      <x:c r="E2" s="21" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:5">
+    <x:row r="3" spans="1:5" s="24" customFormat="1" ht="30" customHeight="1">
       <x:c r="A3" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -740,7 +804,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="E4" s="9" t="n">
-        <x:v>2000</x:v>
+        <x:v>600</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -751,43 +815,43 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C5" s="7" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D5" s="8" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E5" s="9" t="n">
-        <x:v>3100</x:v>
+        <x:v>2890</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="10" t="s"/>
       <x:c r="B6" s="11" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C6" s="11" t="n">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D6" s="12" t="s"/>
       <x:c r="E6" s="13" t="n">
-        <x:v>5100</x:v>
+        <x:v>3490</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
-      <x:c r="A7" s="6" t="n">
+      <x:c r="A7" s="14" t="n">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B7" s="7" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C7" s="7" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="D7" s="8" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E7" s="9" t="n">
-        <x:v>2550</x:v>
+      <x:c r="B7" s="15" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C7" s="15" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D7" s="16" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E7" s="17" t="n">
+        <x:v>1450</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
@@ -795,89 +859,42 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B8" s="7" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C8" s="7" t="n">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C8" s="7" t="n">
-        <x:v>5</x:v>
-      </x:c>
       <x:c r="D8" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E8" s="9" t="n">
-        <x:v>4140</x:v>
+        <x:v>5530</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="10" t="s"/>
       <x:c r="B9" s="11" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C9" s="11" t="n">
-        <x:v>9</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="12" t="s"/>
       <x:c r="E9" s="13" t="n">
-        <x:v>6690</x:v>
+        <x:v>6980</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
-      <x:c r="A10" s="6" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B10" s="7" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C10" s="7" t="n">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="D10" s="8" t="s">
+      <x:c r="A10" s="18" t="s"/>
+      <x:c r="B10" s="18" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C10" s="18" t="n">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E10" s="9" t="n">
-        <x:v>8440</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="6" t="n">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B11" s="7" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C11" s="7" t="n">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D11" s="8" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E11" s="9" t="n">
-        <x:v>9735</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="14" t="s"/>
-      <x:c r="B12" s="15" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C12" s="15" t="n">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="D12" s="16" t="s"/>
-      <x:c r="E12" s="17" t="n">
-        <x:v>18175</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="11" t="s"/>
-      <x:c r="B13" s="11" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C13" s="11" t="n">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="D13" s="12" t="s"/>
-      <x:c r="E13" s="18" t="n">
-        <x:v>29965</x:v>
+      <x:c r="D10" s="19" t="s"/>
+      <x:c r="E10" s="20" t="n">
+        <x:v>10470</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>